<commit_message>
started FEMM sim write-up, finished switch sim write-up
</commit_message>
<xml_diff>
--- a/FEMM Simulations/Data/DimensionSweep 2019_10_23 11_51/60uH_Dimensions.xlsx
+++ b/FEMM Simulations/Data/DimensionSweep 2019_10_23 11_51/60uH_Dimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekultho\Documents\Personal\CG 490\FEMM Simulations\Data\DimensionSweep 2019_10_23 11_51\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3305B5A-6E66-4576-BC19-3FFFA0CD5EE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64A998F-02BA-4E3E-B641-5E43ABC5760D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="660" yWindow="600" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1951,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="A15:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>